<commit_message>
Integracion de nuevos modulos en el backend y nuevos endpoints
</commit_message>
<xml_diff>
--- a/Documentacion/Product Backlog/Product Backlog Kevin Urbano-6523.xlsx
+++ b/Documentacion/Product Backlog/Product Backlog Kevin Urbano-6523.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APP2\Documentacion\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9052BF53-5747-4565-900C-7868775B2258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4DAC02-E2F6-4D03-912F-FF03ACD21220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="163">
   <si>
     <t>Columna</t>
   </si>
@@ -229,9 +229,6 @@
   </si>
   <si>
     <t>HT12</t>
-  </si>
-  <si>
-    <t>Gestión carrito</t>
   </si>
   <si>
     <t>HT11</t>
@@ -1253,7 +1250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="156" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="156" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="G5" sqref="G5:H23"/>
     </sheetView>
   </sheetViews>
@@ -1371,7 +1368,7 @@
       <c r="C5" s="21"/>
       <c r="D5" s="20"/>
       <c r="E5" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" s="8">
         <v>2</v>
@@ -1391,13 +1388,13 @@
         <v>43</v>
       </c>
       <c r="P5" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q5" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="Q5" s="16" t="s">
+      <c r="R5" s="16" t="s">
         <v>70</v>
-      </c>
-      <c r="R5" s="16" t="s">
-        <v>71</v>
       </c>
       <c r="S5"/>
       <c r="T5"/>
@@ -1410,7 +1407,7 @@
       <c r="C6" s="21"/>
       <c r="D6" s="20"/>
       <c r="E6" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F6" s="8">
         <v>4</v>
@@ -1433,7 +1430,7 @@
         <v>15</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R6" s="40">
         <v>45776</v>
@@ -1449,7 +1446,7 @@
       <c r="C7" s="21"/>
       <c r="D7" s="20"/>
       <c r="E7" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" s="8">
         <v>3</v>
@@ -1472,7 +1469,7 @@
         <v>15</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R7" s="40">
         <v>45783</v>
@@ -1488,7 +1485,7 @@
       <c r="C8" s="21"/>
       <c r="D8" s="20"/>
       <c r="E8" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F8" s="8">
         <v>4</v>
@@ -1511,7 +1508,7 @@
         <v>20</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R8" s="40">
         <v>45790</v>
@@ -1527,7 +1524,7 @@
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
       <c r="E9" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F9" s="8">
         <v>3</v>
@@ -1550,7 +1547,7 @@
         <v>20</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R9" s="40">
         <v>45797</v>
@@ -1566,7 +1563,7 @@
       <c r="C10" s="18"/>
       <c r="D10" s="28"/>
       <c r="E10" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F10" s="7">
         <v>2</v>
@@ -1589,7 +1586,7 @@
         <v>25</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R10" s="40">
         <v>45804</v>
@@ -1605,7 +1602,7 @@
       <c r="C11" s="15"/>
       <c r="D11" s="28"/>
       <c r="E11" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F11" s="8">
         <v>3</v>
@@ -1624,7 +1621,7 @@
         <v>25</v>
       </c>
       <c r="Q11" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R11" s="40">
         <v>45811</v>
@@ -1640,7 +1637,7 @@
       <c r="C12" s="28"/>
       <c r="D12" s="27"/>
       <c r="E12" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F12" s="8">
         <v>2</v>
@@ -1659,7 +1656,7 @@
         <v>25</v>
       </c>
       <c r="Q12" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R12" s="40">
         <v>45818</v>
@@ -1675,7 +1672,7 @@
       <c r="C13" s="28"/>
       <c r="D13" s="27"/>
       <c r="E13" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F13" s="8">
         <v>2</v>
@@ -1694,7 +1691,7 @@
         <v>25</v>
       </c>
       <c r="Q13" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R13" s="40">
         <v>45825</v>
@@ -1710,7 +1707,7 @@
       <c r="C14" s="28"/>
       <c r="D14" s="27"/>
       <c r="E14" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F14" s="8">
         <v>5</v>
@@ -1729,7 +1726,7 @@
         <v>30</v>
       </c>
       <c r="Q14" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R14" s="40">
         <v>45832</v>
@@ -1745,7 +1742,7 @@
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
       <c r="E15" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F15" s="7">
         <v>2</v>
@@ -1758,14 +1755,14 @@
       <c r="M15"/>
       <c r="N15"/>
       <c r="O15" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P15" s="16">
         <f>SUM(P6:P14)</f>
         <v>200</v>
       </c>
       <c r="Q15" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R15"/>
       <c r="S15"/>
@@ -1779,7 +1776,7 @@
       <c r="C16" s="29"/>
       <c r="D16" s="28"/>
       <c r="E16" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F16" s="8">
         <v>3</v>
@@ -1833,7 +1830,7 @@
       <c r="C17" s="29"/>
       <c r="D17" s="28"/>
       <c r="E17" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F17" s="8">
         <v>3</v>
@@ -1887,7 +1884,7 @@
       <c r="C18" s="29"/>
       <c r="D18" s="28"/>
       <c r="E18" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F18" s="8">
         <v>5</v>
@@ -1941,7 +1938,7 @@
       <c r="C19" s="29"/>
       <c r="D19" s="28"/>
       <c r="E19" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F19" s="8">
         <v>5</v>
@@ -1995,7 +1992,7 @@
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
       <c r="E20" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F20" s="9">
         <v>2</v>
@@ -2050,7 +2047,7 @@
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
       <c r="E21" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F21" s="7">
         <v>5</v>
@@ -2114,7 +2111,7 @@
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
       <c r="E22" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F22" s="9">
         <v>3</v>
@@ -2177,7 +2174,7 @@
       <c r="C23" s="15"/>
       <c r="D23" s="20"/>
       <c r="E23" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F23" s="9">
         <v>5</v>
@@ -6530,8 +6527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15781DD-9345-4FBC-BA12-9DDB8B35BAA9}">
   <dimension ref="B1:E91"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6570,10 +6567,10 @@
         <v>31</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="28">
         <v>2</v>
@@ -6584,10 +6581,10 @@
         <v>32</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5" s="28">
         <v>2</v>
@@ -6598,10 +6595,10 @@
         <v>33</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" s="28">
         <v>2</v>
@@ -6609,13 +6606,13 @@
     </row>
     <row r="7" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7" s="28">
         <v>2</v>
@@ -6651,13 +6648,13 @@
     </row>
     <row r="11" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E11" s="28">
         <v>3</v>
@@ -6668,10 +6665,10 @@
         <v>21</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E12" s="28">
         <v>3</v>
@@ -6679,13 +6676,13 @@
     </row>
     <row r="13" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E13" s="28">
         <v>3</v>
@@ -6724,10 +6721,10 @@
         <v>45</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E17" s="28">
         <v>2</v>
@@ -6738,10 +6735,10 @@
         <v>35</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E18" s="28">
         <v>2</v>
@@ -6749,13 +6746,13 @@
     </row>
     <row r="19" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E19" s="28">
         <v>2</v>
@@ -6766,10 +6763,10 @@
         <v>22</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E20" s="28">
         <v>2</v>
@@ -6805,13 +6802,13 @@
     </row>
     <row r="24" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="27" t="s">
-        <v>87</v>
-      </c>
       <c r="D24" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E24" s="28">
         <v>4</v>
@@ -6822,7 +6819,7 @@
         <v>34</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D25" s="27" t="s">
         <v>44</v>
@@ -6836,10 +6833,10 @@
         <v>56</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E26" s="28">
         <v>2</v>
@@ -6847,13 +6844,13 @@
     </row>
     <row r="27" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E27" s="28">
         <v>3</v>
@@ -6861,13 +6858,13 @@
     </row>
     <row r="28" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E28" s="28">
         <v>3</v>
@@ -6875,13 +6872,13 @@
     </row>
     <row r="29" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E29" s="28">
         <v>3</v>
@@ -6917,13 +6914,13 @@
     </row>
     <row r="33" spans="2:5" s="41" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E33" s="28">
         <v>2</v>
@@ -6934,10 +6931,10 @@
         <v>60</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D34" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E34" s="28">
         <v>2</v>
@@ -6945,13 +6942,13 @@
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E35" s="28">
         <v>3</v>
@@ -6959,13 +6956,13 @@
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E36" s="28">
         <v>3</v>
@@ -6973,13 +6970,13 @@
     </row>
     <row r="37" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B37" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E37" s="28">
         <v>3</v>
@@ -6987,13 +6984,13 @@
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E38" s="28">
         <v>3</v>
@@ -7035,13 +7032,13 @@
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E43" s="28">
         <v>3</v>
@@ -7049,13 +7046,13 @@
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E44" s="28">
         <v>3</v>
@@ -7063,13 +7060,13 @@
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E45" s="28">
         <v>3</v>
@@ -7077,13 +7074,13 @@
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E46" s="28">
         <v>3</v>
@@ -7091,13 +7088,13 @@
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D47" s="27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E47" s="28">
         <v>3</v>
@@ -7105,13 +7102,13 @@
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C48" s="27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D48" s="27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E48" s="28">
         <v>3</v>
@@ -7119,13 +7116,13 @@
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E49" s="28">
         <v>3</v>
@@ -7167,13 +7164,13 @@
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C54" s="30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D54" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E54" s="28">
         <v>3</v>
@@ -7181,13 +7178,13 @@
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C55" s="30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E55" s="28">
         <v>3</v>
@@ -7195,13 +7192,13 @@
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C56" s="30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E56" s="28">
         <v>3</v>
@@ -7209,13 +7206,13 @@
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C57" s="30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D57" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E57" s="28">
         <v>3</v>
@@ -7223,13 +7220,13 @@
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C58" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D58" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E58" s="28">
         <v>3</v>
@@ -7237,13 +7234,13 @@
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C59" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D59" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E59" s="28">
         <v>3</v>
@@ -7279,13 +7276,13 @@
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C63" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="D63" s="27" t="s">
-        <v>61</v>
+        <v>131</v>
+      </c>
+      <c r="D63" s="30" t="s">
+        <v>131</v>
       </c>
       <c r="E63" s="28">
         <v>4</v>
@@ -7293,13 +7290,13 @@
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C64" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="D64" s="27" t="s">
-        <v>61</v>
+        <v>132</v>
+      </c>
+      <c r="D64" s="30" t="s">
+        <v>132</v>
       </c>
       <c r="E64" s="28">
         <v>4</v>
@@ -7307,13 +7304,13 @@
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C65" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="D65" s="27" t="s">
-        <v>61</v>
+        <v>133</v>
+      </c>
+      <c r="D65" s="30" t="s">
+        <v>133</v>
       </c>
       <c r="E65" s="28">
         <v>4</v>
@@ -7321,13 +7318,13 @@
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C66" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="D66" s="27" t="s">
         <v>138</v>
-      </c>
-      <c r="D66" s="27" t="s">
-        <v>139</v>
       </c>
       <c r="E66" s="28">
         <v>4</v>
@@ -7335,13 +7332,13 @@
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C67" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D67" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E67" s="28">
         <v>4</v>
@@ -7349,13 +7346,13 @@
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C68" s="30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D68" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E68" s="28">
         <v>4</v>
@@ -7391,13 +7388,13 @@
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C72" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D72" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E72" s="28">
         <v>5</v>
@@ -7405,13 +7402,13 @@
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C73" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D73" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E73" s="28">
         <v>5</v>
@@ -7419,13 +7416,13 @@
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C74" s="30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D74" s="30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E74" s="28">
         <v>5</v>
@@ -7433,13 +7430,13 @@
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" s="27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C75" s="30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D75" s="30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E75" s="28">
         <v>5</v>
@@ -7447,13 +7444,13 @@
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C76" s="30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D76" s="30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E76" s="28">
         <v>5</v>
@@ -7461,13 +7458,13 @@
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C77" s="30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D77" s="30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E77" s="28">
         <v>5</v>
@@ -7503,13 +7500,13 @@
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="C81" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="C81" s="30" t="s">
-        <v>155</v>
-      </c>
       <c r="D81" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E81" s="28">
         <v>5</v>
@@ -7517,13 +7514,13 @@
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="C82" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="C82" s="30" t="s">
-        <v>157</v>
-      </c>
       <c r="D82" s="30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E82" s="28">
         <v>5</v>
@@ -7559,13 +7556,13 @@
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C86" s="30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D86" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E86" s="28">
         <v>4</v>
@@ -7573,13 +7570,13 @@
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C87" s="37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D87" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E87" s="28">
         <v>3</v>
@@ -7587,13 +7584,13 @@
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" s="27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C88" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D88" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E88" s="28">
         <v>5</v>

</xml_diff>